<commit_message>
added the logs code---
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata/TestData.xlsx
+++ b/target/test-classes/testdata/TestData.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\IdeaProjects\DDT web Hybrid framework Excel\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apoorva\IdeaProjects\DDT-web-Hybrid-framework-Excel\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96C01B1-CBD0-4ADF-B537-51F3130F71A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DAC837-37D8-422F-8284-4E7D6CB54837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9375" yWindow="3930" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Username</t>
   </si>
@@ -37,13 +40,115 @@
   </si>
   <si>
     <t>demo</t>
+  </si>
+  <si>
+    <t>Solutions</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Locations</t>
+  </si>
+  <si>
+    <t>Admin Page</t>
+  </si>
+  <si>
+    <t>About Us</t>
+  </si>
+  <si>
+    <t>Nav bar</t>
+  </si>
+  <si>
+    <t>Serial No.</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Balance*</t>
+  </si>
+  <si>
+    <t>Available Amount</t>
+  </si>
+  <si>
+    <t>Account Services</t>
+  </si>
+  <si>
+    <t>Open New Account</t>
+  </si>
+  <si>
+    <t>Accounts Overview</t>
+  </si>
+  <si>
+    <t>Transfer Funds</t>
+  </si>
+  <si>
+    <t>Bill Pay</t>
+  </si>
+  <si>
+    <t>Find Transactions</t>
+  </si>
+  <si>
+    <t>Update Contact Info</t>
+  </si>
+  <si>
+    <t>Request Loan</t>
+  </si>
+  <si>
+    <t>Log Out</t>
+  </si>
+  <si>
+    <t>Home|</t>
+  </si>
+  <si>
+    <t>About Us|</t>
+  </si>
+  <si>
+    <t>Services|</t>
+  </si>
+  <si>
+    <t>Products|</t>
+  </si>
+  <si>
+    <t>Locations|</t>
+  </si>
+  <si>
+    <t>Forum|</t>
+  </si>
+  <si>
+    <t>Site Map|</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
+  </si>
+  <si>
+    <t>PageTitle</t>
+  </si>
+  <si>
+    <t>ParaBank | Register for Free Online Account Access</t>
+  </si>
+  <si>
+    <t>Signing up is easy!</t>
+  </si>
+  <si>
+    <t>Signup Form</t>
+  </si>
+  <si>
+    <t>ParaBank | Welcome | Online Banking</t>
+  </si>
+  <si>
+    <t>PageTitle2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,16 +163,59 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF003399"/>
+      <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF305E5C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3979AA"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB9C9FE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -75,13 +223,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFD3DDFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,32 +546,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="42" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089BBC2D-3268-4086-9D25-2495A915A5DD}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="13" max="13" width="24.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA75E8CD-0594-41B6-A3CB-AFDCF1CCEF7F}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA84324-57B3-46B8-8173-137DF167ECA9}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>